<commit_message>
Added only prices and random assignment algorithms to coordinator
Signed-off-by: aytugy <aytug.yavuzer@rwth-aachen.de>
</commit_message>
<xml_diff>
--- a/external/datafev/outputs/mcsysytem_output.xlsx
+++ b/external/datafev/outputs/mcsysytem_output.xlsx
@@ -45,7 +45,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -71,13 +71,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin"/>
-      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border>
@@ -465,7 +458,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -541,7 +534,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>ev001</t>
+          <t>ev1</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -551,7 +544,7 @@
         <v>44569.29513888889</v>
       </c>
       <c r="E2" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -561,17 +554,17 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>cu_1_c</t>
+          <t>cu_2_a</t>
         </is>
       </c>
       <c r="I2" s="2" t="n">
         <v>44569.33680555555</v>
       </c>
       <c r="J2" t="n">
-        <v>0.7499999999999998</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="K2" t="n">
-        <v>21.99999999999999</v>
+        <v>19.99999999999998</v>
       </c>
       <c r="L2" t="n">
         <v>0</v>
@@ -586,7 +579,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>ev002</t>
+          <t>ev2</t>
         </is>
       </c>
       <c r="C3" t="n">
@@ -596,7 +589,7 @@
         <v>44569.29861111111</v>
       </c>
       <c r="E3" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -606,17 +599,17 @@
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>cu_1_d</t>
+          <t>cu_2_b</t>
         </is>
       </c>
       <c r="I3" s="2" t="n">
         <v>44569.34027777778</v>
       </c>
       <c r="J3" t="n">
-        <v>0.7499999999999998</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="K3" t="n">
-        <v>21.99999999999999</v>
+        <v>19.99999999999998</v>
       </c>
       <c r="L3" t="n">
         <v>0</v>
@@ -631,7 +624,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>ev003</t>
+          <t>ev3</t>
         </is>
       </c>
       <c r="C4" t="n">
@@ -641,7 +634,7 @@
         <v>44569.30208333334</v>
       </c>
       <c r="E4" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -651,23 +644,23 @@
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>cu_1_e</t>
+          <t>cu_3_a</t>
         </is>
       </c>
       <c r="I4" s="2" t="n">
         <v>44569.34375</v>
       </c>
       <c r="J4" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="K4" t="n">
-        <v>31.99999999999999</v>
+        <v>19.99999999999998</v>
       </c>
       <c r="L4" t="n">
         <v>0</v>
       </c>
       <c r="M4" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
@@ -676,7 +669,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>ev004</t>
+          <t>ev4</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -686,7 +679,7 @@
         <v>44569.30555555555</v>
       </c>
       <c r="E5" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -696,23 +689,23 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>cu_1_f</t>
+          <t>cu_3_b</t>
         </is>
       </c>
       <c r="I5" s="2" t="n">
         <v>44569.34722222222</v>
       </c>
       <c r="J5" t="n">
-        <v>0.9999999999999999</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="K5" t="n">
-        <v>31.99999999999999</v>
+        <v>19.99999999999998</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
       </c>
       <c r="M5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -721,7 +714,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>ev005</t>
+          <t>ev5</t>
         </is>
       </c>
       <c r="C6" t="n">
@@ -731,7 +724,7 @@
         <v>44569.30902777778</v>
       </c>
       <c r="E6" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -741,23 +734,23 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>cu_1_a</t>
+          <t>cu_4_a</t>
         </is>
       </c>
       <c r="I6" s="2" t="n">
         <v>44569.35069444445</v>
       </c>
       <c r="J6" t="n">
-        <v>0.4749999999999998</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="K6" t="n">
-        <v>10.99999999999999</v>
+        <v>19.99999999999998</v>
       </c>
       <c r="L6" t="n">
         <v>0</v>
       </c>
       <c r="M6" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
@@ -766,7 +759,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>ev006</t>
+          <t>ev6</t>
         </is>
       </c>
       <c r="C7" t="n">
@@ -776,7 +769,7 @@
         <v>44569.3125</v>
       </c>
       <c r="E7" t="n">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -786,113 +779,23 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>cu_1_b</t>
+          <t>cu_4_b</t>
         </is>
       </c>
       <c r="I7" s="2" t="n">
         <v>44569.35416666666</v>
       </c>
       <c r="J7" t="n">
-        <v>0.4749999999999998</v>
+        <v>0.9999999999999996</v>
       </c>
       <c r="K7" t="n">
-        <v>10.99999999999999</v>
+        <v>19.99999999999998</v>
       </c>
       <c r="L7" t="n">
         <v>0</v>
       </c>
       <c r="M7" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>ev007</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>40</v>
-      </c>
-      <c r="D8" s="2" t="n">
-        <v>44569.31597222222</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F8" t="n">
-        <v>0</v>
-      </c>
-      <c r="G8" t="n">
-        <v>0</v>
-      </c>
-      <c r="H8" t="inlineStr">
-        <is>
-          <t>cu_1_g</t>
-        </is>
-      </c>
-      <c r="I8" s="2" t="n">
-        <v>44569.35763888889</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.9999999999999998</v>
-      </c>
-      <c r="K8" t="n">
-        <v>31.99999999999999</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0</v>
-      </c>
-      <c r="M8" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>ev008</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>40</v>
-      </c>
-      <c r="D9" s="2" t="n">
-        <v>44569.31944444445</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F9" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" t="inlineStr">
-        <is>
-          <t>cu_1_h</t>
-        </is>
-      </c>
-      <c r="I9" s="2" t="n">
-        <v>44569.36111111111</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.9999999999999998</v>
-      </c>
-      <c r="K9" t="n">
-        <v>31.99999999999999</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -922,11 +825,23 @@
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="I1" s="1" t="n"/>
     </row>
     <row r="2">
@@ -943,32 +858,32 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_c</t>
+          <t>cu_2_a</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_d</t>
+          <t>cu_2_b</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_e</t>
+          <t>cu_3_a</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_f</t>
+          <t>cu_3_b</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_g</t>
+          <t>cu_4_a</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_h</t>
+          <t>cu_4_b</t>
         </is>
       </c>
     </row>
@@ -1012,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1041,10 +956,10 @@
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E6" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -1070,13 +985,13 @@
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E7" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F7" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G7" t="n">
         <v>0</v>
@@ -1099,16 +1014,16 @@
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E8" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F8" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G8" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="H8" t="n">
         <v>0</v>
@@ -1122,25 +1037,25 @@
         <v>44569.30902777778</v>
       </c>
       <c r="B9" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E9" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F9" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G9" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -1151,28 +1066,28 @@
         <v>44569.3125</v>
       </c>
       <c r="B10" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E10" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F10" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G10" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11">
@@ -1180,28 +1095,28 @@
         <v>44569.31597222222</v>
       </c>
       <c r="B11" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E11" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F11" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G11" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="H11" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12">
@@ -1209,28 +1124,28 @@
         <v>44569.31944444445</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E12" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F12" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="G12" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="H12" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="I12" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13">
@@ -1238,28 +1153,28 @@
         <v>44569.32291666666</v>
       </c>
       <c r="B13" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E13" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F13" t="n">
-        <v>53.99999999999991</v>
+        <v>20</v>
       </c>
       <c r="G13" t="n">
-        <v>55</v>
+        <v>20</v>
       </c>
       <c r="H13" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
       <c r="I13" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="14">
@@ -1267,28 +1182,28 @@
         <v>44569.32638888889</v>
       </c>
       <c r="B14" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E14" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G14" t="n">
-        <v>53.99999999999991</v>
+        <v>20</v>
       </c>
       <c r="H14" t="n">
-        <v>53.99999999999991</v>
+        <v>20</v>
       </c>
       <c r="I14" t="n">
-        <v>110</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15">
@@ -1296,28 +1211,28 @@
         <v>44569.32986111111</v>
       </c>
       <c r="B15" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E15" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H15" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I15" t="n">
-        <v>53.99999999999991</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16">
@@ -1325,28 +1240,28 @@
         <v>44569.33333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E16" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17">
@@ -1354,28 +1269,28 @@
         <v>44569.33680555555</v>
       </c>
       <c r="B17" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I17" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18">
@@ -1383,10 +1298,10 @@
         <v>44569.34027777778</v>
       </c>
       <c r="B18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -1395,16 +1310,16 @@
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="G18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19">
@@ -1412,10 +1327,10 @@
         <v>44569.34375</v>
       </c>
       <c r="B19" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -1427,13 +1342,13 @@
         <v>0</v>
       </c>
       <c r="G19" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H19" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I19" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -1441,10 +1356,10 @@
         <v>44569.34722222222</v>
       </c>
       <c r="B20" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -1459,10 +1374,10 @@
         <v>0</v>
       </c>
       <c r="H20" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="I20" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21">
@@ -1473,7 +1388,7 @@
         <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -1491,7 +1406,7 @@
         <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22">
@@ -2742,8 +2657,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2755,7 +2673,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2769,6 +2687,21 @@
           <t>1</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
@@ -2777,13 +2710,31 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
         <v>44569.29513888889</v>
       </c>
       <c r="B3" t="n">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>20</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -2791,7 +2742,16 @@
         <v>44569.29861111111</v>
       </c>
       <c r="B4" t="n">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>40</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -2799,7 +2759,16 @@
         <v>44569.30208333334</v>
       </c>
       <c r="B5" t="n">
-        <v>99</v>
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>40</v>
+      </c>
+      <c r="D5" t="n">
+        <v>20</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -2807,7 +2776,16 @@
         <v>44569.30555555555</v>
       </c>
       <c r="B6" t="n">
-        <v>154</v>
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>40</v>
+      </c>
+      <c r="D6" t="n">
+        <v>40</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -2815,7 +2793,16 @@
         <v>44569.30902777778</v>
       </c>
       <c r="B7" t="n">
-        <v>165</v>
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>40</v>
+      </c>
+      <c r="D7" t="n">
+        <v>40</v>
+      </c>
+      <c r="E7" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="8">
@@ -2823,7 +2810,16 @@
         <v>44569.3125</v>
       </c>
       <c r="B8" t="n">
-        <v>176</v>
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>40</v>
+      </c>
+      <c r="D8" t="n">
+        <v>40</v>
+      </c>
+      <c r="E8" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="9">
@@ -2831,7 +2827,16 @@
         <v>44569.31597222222</v>
       </c>
       <c r="B9" t="n">
-        <v>286</v>
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>40</v>
+      </c>
+      <c r="D9" t="n">
+        <v>40</v>
+      </c>
+      <c r="E9" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="10">
@@ -2839,7 +2844,16 @@
         <v>44569.31944444445</v>
       </c>
       <c r="B10" t="n">
-        <v>396</v>
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>40</v>
+      </c>
+      <c r="D10" t="n">
+        <v>40</v>
+      </c>
+      <c r="E10" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="11">
@@ -2847,7 +2861,16 @@
         <v>44569.32291666666</v>
       </c>
       <c r="B11" t="n">
-        <v>394.9999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>40</v>
+      </c>
+      <c r="D11" t="n">
+        <v>40</v>
+      </c>
+      <c r="E11" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="12">
@@ -2855,7 +2878,16 @@
         <v>44569.32638888889</v>
       </c>
       <c r="B12" t="n">
-        <v>283.9999999999998</v>
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>40</v>
+      </c>
+      <c r="D12" t="n">
+        <v>40</v>
+      </c>
+      <c r="E12" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="13">
@@ -2863,7 +2895,16 @@
         <v>44569.32986111111</v>
       </c>
       <c r="B13" t="n">
-        <v>119.9999999999999</v>
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>40</v>
+      </c>
+      <c r="D13" t="n">
+        <v>40</v>
+      </c>
+      <c r="E13" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="14">
@@ -2871,7 +2912,16 @@
         <v>44569.33333333334</v>
       </c>
       <c r="B14" t="n">
-        <v>66</v>
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>40</v>
+      </c>
+      <c r="D14" t="n">
+        <v>40</v>
+      </c>
+      <c r="E14" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="15">
@@ -2879,7 +2929,16 @@
         <v>44569.33680555555</v>
       </c>
       <c r="B15" t="n">
-        <v>44</v>
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>20</v>
+      </c>
+      <c r="D15" t="n">
+        <v>40</v>
+      </c>
+      <c r="E15" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="16">
@@ -2887,7 +2946,16 @@
         <v>44569.34027777778</v>
       </c>
       <c r="B16" t="n">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0</v>
+      </c>
+      <c r="D16" t="n">
+        <v>40</v>
+      </c>
+      <c r="E16" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="17">
@@ -2895,7 +2963,16 @@
         <v>44569.34375</v>
       </c>
       <c r="B17" t="n">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>20</v>
+      </c>
+      <c r="E17" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="18">
@@ -2903,7 +2980,16 @@
         <v>44569.34722222222</v>
       </c>
       <c r="B18" t="n">
-        <v>22</v>
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="19">
@@ -2911,7 +2997,16 @@
         <v>44569.35069444445</v>
       </c>
       <c r="B19" t="n">
-        <v>11</v>
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>20</v>
       </c>
     </row>
     <row r="20">
@@ -2921,6 +3016,15 @@
       <c r="B20" t="n">
         <v>0</v>
       </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="3" t="n">
@@ -2929,6 +3033,15 @@
       <c r="B21" t="n">
         <v>0</v>
       </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="3" t="n">
@@ -2937,6 +3050,15 @@
       <c r="B22" t="n">
         <v>0</v>
       </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="3" t="n">
@@ -2945,6 +3067,15 @@
       <c r="B23" t="n">
         <v>0</v>
       </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
@@ -2953,6 +3084,15 @@
       <c r="B24" t="n">
         <v>0</v>
       </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
@@ -2961,6 +3101,15 @@
       <c r="B25" t="n">
         <v>0</v>
       </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="n">
@@ -2969,6 +3118,15 @@
       <c r="B26" t="n">
         <v>0</v>
       </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="n">
@@ -2977,6 +3135,15 @@
       <c r="B27" t="n">
         <v>0</v>
       </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="n">
@@ -2985,6 +3152,15 @@
       <c r="B28" t="n">
         <v>0</v>
       </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="n">
@@ -2993,6 +3169,15 @@
       <c r="B29" t="n">
         <v>0</v>
       </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="n">
@@ -3001,6 +3186,15 @@
       <c r="B30" t="n">
         <v>0</v>
       </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="n">
@@ -3009,6 +3203,15 @@
       <c r="B31" t="n">
         <v>0</v>
       </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="n">
@@ -3017,6 +3220,15 @@
       <c r="B32" t="n">
         <v>0</v>
       </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="n">
@@ -3025,6 +3237,15 @@
       <c r="B33" t="n">
         <v>0</v>
       </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="n">
@@ -3033,6 +3254,15 @@
       <c r="B34" t="n">
         <v>0</v>
       </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="n">
@@ -3041,6 +3271,15 @@
       <c r="B35" t="n">
         <v>0</v>
       </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="n">
@@ -3049,6 +3288,15 @@
       <c r="B36" t="n">
         <v>0</v>
       </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="n">
@@ -3057,6 +3305,15 @@
       <c r="B37" t="n">
         <v>0</v>
       </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="n">
@@ -3065,6 +3322,15 @@
       <c r="B38" t="n">
         <v>0</v>
       </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="n">
@@ -3073,6 +3339,15 @@
       <c r="B39" t="n">
         <v>0</v>
       </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="n">
@@ -3081,6 +3356,15 @@
       <c r="B40" t="n">
         <v>0</v>
       </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="n">
@@ -3089,6 +3373,15 @@
       <c r="B41" t="n">
         <v>0</v>
       </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="n">
@@ -3097,6 +3390,15 @@
       <c r="B42" t="n">
         <v>0</v>
       </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="n">
@@ -3105,6 +3407,15 @@
       <c r="B43" t="n">
         <v>0</v>
       </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="n">
@@ -3113,6 +3424,15 @@
       <c r="B44" t="n">
         <v>0</v>
       </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="n">
@@ -3121,6 +3441,15 @@
       <c r="B45" t="n">
         <v>0</v>
       </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="n">
@@ -3129,6 +3458,15 @@
       <c r="B46" t="n">
         <v>0</v>
       </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="n">
@@ -3137,6 +3475,15 @@
       <c r="B47" t="n">
         <v>0</v>
       </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="n">
@@ -3145,6 +3492,15 @@
       <c r="B48" t="n">
         <v>0</v>
       </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="n">
@@ -3153,6 +3509,15 @@
       <c r="B49" t="n">
         <v>0</v>
       </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="n">
@@ -3161,6 +3526,15 @@
       <c r="B50" t="n">
         <v>0</v>
       </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="n">
@@ -3169,6 +3543,15 @@
       <c r="B51" t="n">
         <v>0</v>
       </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="n">
@@ -3177,6 +3560,15 @@
       <c r="B52" t="n">
         <v>0</v>
       </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="n">
@@ -3185,6 +3577,15 @@
       <c r="B53" t="n">
         <v>0</v>
       </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="n">
@@ -3193,6 +3594,15 @@
       <c r="B54" t="n">
         <v>0</v>
       </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="n">
@@ -3201,6 +3611,15 @@
       <c r="B55" t="n">
         <v>0</v>
       </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="n">
@@ -3209,6 +3628,15 @@
       <c r="B56" t="n">
         <v>0</v>
       </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="n">
@@ -3217,6 +3645,15 @@
       <c r="B57" t="n">
         <v>0</v>
       </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="n">
@@ -3225,6 +3662,15 @@
       <c r="B58" t="n">
         <v>0</v>
       </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="n">
@@ -3233,6 +3679,15 @@
       <c r="B59" t="n">
         <v>0</v>
       </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="n">
@@ -3241,6 +3696,15 @@
       <c r="B60" t="n">
         <v>0</v>
       </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="n">
@@ -3249,12 +3713,30 @@
       <c r="B61" t="n">
         <v>0</v>
       </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="n">
         <v>44569.5</v>
       </c>
       <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3285,11 +3767,23 @@
         </is>
       </c>
       <c r="C1" s="1" t="n"/>
-      <c r="D1" s="1" t="n"/>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
       <c r="E1" s="1" t="n"/>
-      <c r="F1" s="1" t="n"/>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
       <c r="G1" s="1" t="n"/>
-      <c r="H1" s="1" t="n"/>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
       <c r="I1" s="1" t="n"/>
     </row>
     <row r="2">
@@ -3306,32 +3800,32 @@
       </c>
       <c r="D2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_c</t>
+          <t>cu_2_a</t>
         </is>
       </c>
       <c r="E2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_d</t>
+          <t>cu_2_b</t>
         </is>
       </c>
       <c r="F2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_e</t>
+          <t>cu_3_a</t>
         </is>
       </c>
       <c r="G2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_f</t>
+          <t>cu_3_b</t>
         </is>
       </c>
       <c r="H2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_g</t>
+          <t>cu_4_a</t>
         </is>
       </c>
       <c r="I2" s="1" t="inlineStr">
         <is>
-          <t>cu_1_h</t>
+          <t>cu_4_b</t>
         </is>
       </c>
     </row>
@@ -3485,7 +3979,7 @@
         <v>44569.30902777778</v>
       </c>
       <c r="B9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
@@ -3503,7 +3997,7 @@
         <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I9" t="n">
         <v>0</v>
@@ -3514,10 +4008,10 @@
         <v>44569.3125</v>
       </c>
       <c r="B10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D10" t="n">
         <v>1</v>
@@ -3532,10 +4026,10 @@
         <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -3543,10 +4037,10 @@
         <v>44569.31597222222</v>
       </c>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D11" t="n">
         <v>1</v>
@@ -3564,7 +4058,7 @@
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
@@ -3572,10 +4066,10 @@
         <v>44569.31944444445</v>
       </c>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D12" t="n">
         <v>1</v>
@@ -3601,10 +4095,10 @@
         <v>44569.32291666666</v>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D13" t="n">
         <v>1</v>
@@ -3630,10 +4124,10 @@
         <v>44569.32638888889</v>
       </c>
       <c r="B14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D14" t="n">
         <v>1</v>
@@ -3659,10 +4153,10 @@
         <v>44569.32986111111</v>
       </c>
       <c r="B15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D15" t="n">
         <v>1</v>
@@ -3688,10 +4182,10 @@
         <v>44569.33333333334</v>
       </c>
       <c r="B16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16" t="n">
         <v>1</v>
@@ -3717,10 +4211,10 @@
         <v>44569.33680555555</v>
       </c>
       <c r="B17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D17" t="n">
         <v>1</v>
@@ -3746,10 +4240,10 @@
         <v>44569.34027777778</v>
       </c>
       <c r="B18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C18" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D18" t="n">
         <v>0</v>
@@ -3775,10 +4269,10 @@
         <v>44569.34375</v>
       </c>
       <c r="B19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D19" t="n">
         <v>0</v>
@@ -3804,10 +4298,10 @@
         <v>44569.34722222222</v>
       </c>
       <c r="B20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C20" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D20" t="n">
         <v>0</v>
@@ -3833,10 +4327,10 @@
         <v>44569.35069444445</v>
       </c>
       <c r="B21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C21" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D21" t="n">
         <v>0</v>
@@ -3865,7 +4359,7 @@
         <v>0</v>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D22" t="n">
         <v>0</v>
@@ -3880,7 +4374,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22" t="n">
         <v>1</v>
@@ -3909,10 +4403,10 @@
         <v>0</v>
       </c>
       <c r="H23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -3941,7 +4435,7 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -5105,8 +5599,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="D1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5118,7 +5615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:E62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5132,6 +5629,21 @@
           <t>1</t>
         </is>
       </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
@@ -5140,13 +5652,31 @@
       <c r="B2" t="n">
         <v>0</v>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
         <v>44569.29513888889</v>
       </c>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -5154,7 +5684,16 @@
         <v>44569.29861111111</v>
       </c>
       <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
         <v>2</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -5162,7 +5701,16 @@
         <v>44569.30208333334</v>
       </c>
       <c r="B5" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -5170,7 +5718,16 @@
         <v>44569.30555555555</v>
       </c>
       <c r="B6" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>2</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -5178,7 +5735,16 @@
         <v>44569.30902777778</v>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8">
@@ -5186,7 +5752,16 @@
         <v>44569.3125</v>
       </c>
       <c r="B8" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>2</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -5194,7 +5769,16 @@
         <v>44569.31597222222</v>
       </c>
       <c r="B9" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>2</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="10">
@@ -5202,7 +5786,16 @@
         <v>44569.31944444445</v>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C10" t="n">
+        <v>2</v>
+      </c>
+      <c r="D10" t="n">
+        <v>2</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="11">
@@ -5210,7 +5803,16 @@
         <v>44569.32291666666</v>
       </c>
       <c r="B11" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C11" t="n">
+        <v>2</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -5218,7 +5820,16 @@
         <v>44569.32638888889</v>
       </c>
       <c r="B12" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C12" t="n">
+        <v>2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>2</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="13">
@@ -5226,7 +5837,16 @@
         <v>44569.32986111111</v>
       </c>
       <c r="B13" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C13" t="n">
+        <v>2</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -5234,7 +5854,16 @@
         <v>44569.33333333334</v>
       </c>
       <c r="B14" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C14" t="n">
+        <v>2</v>
+      </c>
+      <c r="D14" t="n">
+        <v>2</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -5242,7 +5871,16 @@
         <v>44569.33680555555</v>
       </c>
       <c r="B15" t="n">
-        <v>8</v>
+        <v>0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -5250,7 +5888,16 @@
         <v>44569.34027777778</v>
       </c>
       <c r="B16" t="n">
-        <v>7</v>
+        <v>0</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>2</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -5258,7 +5905,16 @@
         <v>44569.34375</v>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="18">
@@ -5266,7 +5922,16 @@
         <v>44569.34722222222</v>
       </c>
       <c r="B18" t="n">
-        <v>5</v>
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="19">
@@ -5274,7 +5939,16 @@
         <v>44569.35069444445</v>
       </c>
       <c r="B19" t="n">
-        <v>4</v>
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="20">
@@ -5282,7 +5956,16 @@
         <v>44569.35416666666</v>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="21">
@@ -5290,7 +5973,16 @@
         <v>44569.35763888889</v>
       </c>
       <c r="B21" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>0</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0</v>
+      </c>
+      <c r="E21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -5298,7 +5990,16 @@
         <v>44569.36111111111</v>
       </c>
       <c r="B22" t="n">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C22" t="n">
+        <v>0</v>
+      </c>
+      <c r="D22" t="n">
+        <v>0</v>
+      </c>
+      <c r="E22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -5308,6 +6009,15 @@
       <c r="B23" t="n">
         <v>0</v>
       </c>
+      <c r="C23" t="n">
+        <v>0</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0</v>
+      </c>
+      <c r="E23" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="3" t="n">
@@ -5316,6 +6026,15 @@
       <c r="B24" t="n">
         <v>0</v>
       </c>
+      <c r="C24" t="n">
+        <v>0</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="3" t="n">
@@ -5324,6 +6043,15 @@
       <c r="B25" t="n">
         <v>0</v>
       </c>
+      <c r="C25" t="n">
+        <v>0</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="3" t="n">
@@ -5332,6 +6060,15 @@
       <c r="B26" t="n">
         <v>0</v>
       </c>
+      <c r="C26" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="3" t="n">
@@ -5340,6 +6077,15 @@
       <c r="B27" t="n">
         <v>0</v>
       </c>
+      <c r="C27" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="3" t="n">
@@ -5348,6 +6094,15 @@
       <c r="B28" t="n">
         <v>0</v>
       </c>
+      <c r="C28" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="3" t="n">
@@ -5356,6 +6111,15 @@
       <c r="B29" t="n">
         <v>0</v>
       </c>
+      <c r="C29" t="n">
+        <v>0</v>
+      </c>
+      <c r="D29" t="n">
+        <v>0</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="3" t="n">
@@ -5364,6 +6128,15 @@
       <c r="B30" t="n">
         <v>0</v>
       </c>
+      <c r="C30" t="n">
+        <v>0</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="3" t="n">
@@ -5372,6 +6145,15 @@
       <c r="B31" t="n">
         <v>0</v>
       </c>
+      <c r="C31" t="n">
+        <v>0</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="3" t="n">
@@ -5380,6 +6162,15 @@
       <c r="B32" t="n">
         <v>0</v>
       </c>
+      <c r="C32" t="n">
+        <v>0</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="3" t="n">
@@ -5388,6 +6179,15 @@
       <c r="B33" t="n">
         <v>0</v>
       </c>
+      <c r="C33" t="n">
+        <v>0</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="3" t="n">
@@ -5396,6 +6196,15 @@
       <c r="B34" t="n">
         <v>0</v>
       </c>
+      <c r="C34" t="n">
+        <v>0</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="3" t="n">
@@ -5404,6 +6213,15 @@
       <c r="B35" t="n">
         <v>0</v>
       </c>
+      <c r="C35" t="n">
+        <v>0</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="3" t="n">
@@ -5412,6 +6230,15 @@
       <c r="B36" t="n">
         <v>0</v>
       </c>
+      <c r="C36" t="n">
+        <v>0</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="3" t="n">
@@ -5420,6 +6247,15 @@
       <c r="B37" t="n">
         <v>0</v>
       </c>
+      <c r="C37" t="n">
+        <v>0</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="3" t="n">
@@ -5428,6 +6264,15 @@
       <c r="B38" t="n">
         <v>0</v>
       </c>
+      <c r="C38" t="n">
+        <v>0</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="3" t="n">
@@ -5436,6 +6281,15 @@
       <c r="B39" t="n">
         <v>0</v>
       </c>
+      <c r="C39" t="n">
+        <v>0</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="3" t="n">
@@ -5444,6 +6298,15 @@
       <c r="B40" t="n">
         <v>0</v>
       </c>
+      <c r="C40" t="n">
+        <v>0</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="3" t="n">
@@ -5452,6 +6315,15 @@
       <c r="B41" t="n">
         <v>0</v>
       </c>
+      <c r="C41" t="n">
+        <v>0</v>
+      </c>
+      <c r="D41" t="n">
+        <v>0</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="3" t="n">
@@ -5460,6 +6332,15 @@
       <c r="B42" t="n">
         <v>0</v>
       </c>
+      <c r="C42" t="n">
+        <v>0</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="3" t="n">
@@ -5468,6 +6349,15 @@
       <c r="B43" t="n">
         <v>0</v>
       </c>
+      <c r="C43" t="n">
+        <v>0</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="3" t="n">
@@ -5476,6 +6366,15 @@
       <c r="B44" t="n">
         <v>0</v>
       </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="3" t="n">
@@ -5484,6 +6383,15 @@
       <c r="B45" t="n">
         <v>0</v>
       </c>
+      <c r="C45" t="n">
+        <v>0</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" s="3" t="n">
@@ -5492,6 +6400,15 @@
       <c r="B46" t="n">
         <v>0</v>
       </c>
+      <c r="C46" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" t="n">
+        <v>0</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" s="3" t="n">
@@ -5500,6 +6417,15 @@
       <c r="B47" t="n">
         <v>0</v>
       </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" s="3" t="n">
@@ -5508,6 +6434,15 @@
       <c r="B48" t="n">
         <v>0</v>
       </c>
+      <c r="C48" t="n">
+        <v>0</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" s="3" t="n">
@@ -5516,6 +6451,15 @@
       <c r="B49" t="n">
         <v>0</v>
       </c>
+      <c r="C49" t="n">
+        <v>0</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" s="3" t="n">
@@ -5524,6 +6468,15 @@
       <c r="B50" t="n">
         <v>0</v>
       </c>
+      <c r="C50" t="n">
+        <v>0</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" s="3" t="n">
@@ -5532,6 +6485,15 @@
       <c r="B51" t="n">
         <v>0</v>
       </c>
+      <c r="C51" t="n">
+        <v>0</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" s="3" t="n">
@@ -5540,6 +6502,15 @@
       <c r="B52" t="n">
         <v>0</v>
       </c>
+      <c r="C52" t="n">
+        <v>0</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" s="3" t="n">
@@ -5548,6 +6519,15 @@
       <c r="B53" t="n">
         <v>0</v>
       </c>
+      <c r="C53" t="n">
+        <v>0</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" s="3" t="n">
@@ -5556,6 +6536,15 @@
       <c r="B54" t="n">
         <v>0</v>
       </c>
+      <c r="C54" t="n">
+        <v>0</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0</v>
+      </c>
+      <c r="E54" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" s="3" t="n">
@@ -5564,6 +6553,15 @@
       <c r="B55" t="n">
         <v>0</v>
       </c>
+      <c r="C55" t="n">
+        <v>0</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0</v>
+      </c>
+      <c r="E55" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" s="3" t="n">
@@ -5572,6 +6570,15 @@
       <c r="B56" t="n">
         <v>0</v>
       </c>
+      <c r="C56" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" s="3" t="n">
@@ -5580,6 +6587,15 @@
       <c r="B57" t="n">
         <v>0</v>
       </c>
+      <c r="C57" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" s="3" t="n">
@@ -5588,6 +6604,15 @@
       <c r="B58" t="n">
         <v>0</v>
       </c>
+      <c r="C58" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" s="3" t="n">
@@ -5596,6 +6621,15 @@
       <c r="B59" t="n">
         <v>0</v>
       </c>
+      <c r="C59" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0</v>
+      </c>
+      <c r="E59" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" s="3" t="n">
@@ -5604,6 +6638,15 @@
       <c r="B60" t="n">
         <v>0</v>
       </c>
+      <c r="C60" t="n">
+        <v>0</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" s="3" t="n">
@@ -5612,12 +6655,30 @@
       <c r="B61" t="n">
         <v>0</v>
       </c>
+      <c r="C61" t="n">
+        <v>0</v>
+      </c>
+      <c r="D61" t="n">
+        <v>0</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" s="3" t="n">
         <v>44569.5</v>
       </c>
       <c r="B62" t="n">
+        <v>0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>0</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0</v>
+      </c>
+      <c r="E62" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5632,7 +6693,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5674,10 +6735,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>194</v>
+        <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>193.9999999999999</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
@@ -5692,22 +6753,88 @@
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" t="n">
+        <v>39.99999999999996</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>40</v>
+      </c>
+      <c r="C4" t="n">
+        <v>39.99999999999996</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>40</v>
+      </c>
+      <c r="C5" t="n">
+        <v>39.99999999999996</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
           <t>Total</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>194</v>
-      </c>
-      <c r="C3" t="n">
-        <v>193.9999999999999</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="B6" t="n">
+        <v>120</v>
+      </c>
+      <c r="C6" t="n">
+        <v>119.9999999999999</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>